<commit_message>
Updated Schematics and added tL431 datasheet
</commit_message>
<xml_diff>
--- a/LTSimFiles/NiMH Charging Data.xlsx
+++ b/LTSimFiles/NiMH Charging Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10095"/>
   </bookViews>
   <sheets>
     <sheet name="Charging Voltage vs Time" sheetId="2" r:id="rId1"/>
@@ -1546,11 +1546,14 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <webPublishItems count="1">
+    <webPublishItem id="24340" divId="NiMH Charging Data_24340" sourceType="chart" destinationFile="C:\Users\Mark.Smith\Dropbox\personal\SurfnCircuits\BWM_E36_FlashLightHack\LTSimFiles\NiMH Charging Data.mht"/>
+  </webPublishItems>
 </chartsheet>
 </file>
 

</xml_diff>